<commit_message>
Updated templates Descriptions are working
</commit_message>
<xml_diff>
--- a/Data/APNLP_templates.xlsx
+++ b/Data/APNLP_templates.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elisa\Documents\Master\AP Natural Language Processing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elisa\PycharmProjects\Pokerator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBC40E9-1F16-417D-B114-8BE857D8A2D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60959350-4643-4BBE-B23D-D1076091BE6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{10266764-591F-4358-9D03-550F328AD39E}"/>
   </bookViews>
@@ -92,28 +92,28 @@
     <t>a feline</t>
   </si>
   <si>
-    <t>&lt;Pokemon/It&gt; can usually be found in &lt;AtLocation&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Pokemon/It&gt; likes to &lt;CapableOf&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Pokemon/It&gt; hates to &lt;NotDesires&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Pokemon/It&gt; favors &lt;Desires&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Pokemon/It&gt; can &lt;UsedFor&gt; especially well.</t>
-  </si>
-  <si>
-    <t>&lt;Pokemon/It&gt; is a &lt;IsA&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Pokemon/It&gt; can be recognized by its &lt;HasA&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Pokemon/It&gt; is &lt;HasProperty&gt;</t>
+    <t>It can usually be found in &lt;AtLocation&gt;</t>
+  </si>
+  <si>
+    <t>It likes to &lt;CapableOf&gt;</t>
+  </si>
+  <si>
+    <t>It hates to &lt;NotDesires&gt;</t>
+  </si>
+  <si>
+    <t>It favors &lt;Desires&gt;</t>
+  </si>
+  <si>
+    <t>It can &lt;UsedFor&gt; especially well.</t>
+  </si>
+  <si>
+    <t>It is a &lt;IsA&gt;</t>
+  </si>
+  <si>
+    <t>It can be recognized by its &lt;HasA&gt;</t>
+  </si>
+  <si>
+    <t>It is &lt;HasProperty&gt;</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
updated templates with expected pos tag updated conceptnet request to search for fitting relation itself pokedexentrybuilder now making descriptions fitting to pos tagging based on dependency parsing
</commit_message>
<xml_diff>
--- a/Data/APNLP_templates.xlsx
+++ b/Data/APNLP_templates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elisa\PycharmProjects\Pokerator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7094765D-0D3F-4B70-A966-AD3A04403290}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D804DC6-F147-45FB-A97B-F686261A14D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{10266764-591F-4358-9D03-550F328AD39E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Edge types</t>
   </si>
@@ -65,48 +65,12 @@
     <t>HasProperty</t>
   </si>
   <si>
-    <t>Example cat</t>
-  </si>
-  <si>
-    <t>my lap</t>
-  </si>
-  <si>
-    <t>hunt mice</t>
-  </si>
-  <si>
-    <t>be wet</t>
-  </si>
-  <si>
-    <t>milk to drink</t>
-  </si>
-  <si>
-    <t>catch mice</t>
-  </si>
-  <si>
-    <t>feline</t>
-  </si>
-  <si>
-    <t>four legs</t>
-  </si>
-  <si>
-    <t>a feline</t>
-  </si>
-  <si>
     <t>It can usually be found in &lt;AtLocation&gt;</t>
   </si>
   <si>
-    <t>It hates to &lt;NotDesires&gt;</t>
-  </si>
-  <si>
-    <t>It favors &lt;Desires&gt;</t>
-  </si>
-  <si>
     <t>It is a &lt;IsA&gt;</t>
   </si>
   <si>
-    <t>It can be recognized by its &lt;HasA&gt;</t>
-  </si>
-  <si>
     <t>It is &lt;HasProperty&gt;</t>
   </si>
   <si>
@@ -119,9 +83,6 @@
     <t>MadeOf</t>
   </si>
   <si>
-    <t>ReceivesAction</t>
-  </si>
-  <si>
     <t>It is used for &lt;UsedFor&gt;</t>
   </si>
   <si>
@@ -131,7 +92,28 @@
     <t>It is made of &lt;MadeOf&gt;</t>
   </si>
   <si>
-    <t>It can be &lt;ReceivesAction&gt;</t>
+    <t>It has &lt;HasA&gt;</t>
+  </si>
+  <si>
+    <t>It likes &lt;Desires&gt;</t>
+  </si>
+  <si>
+    <t>It hates &lt;NotDesires&gt;</t>
+  </si>
+  <si>
+    <t>Expected POS</t>
+  </si>
+  <si>
+    <t>NOUN</t>
+  </si>
+  <si>
+    <t>VERB</t>
+  </si>
+  <si>
+    <t>NOUN, VERB</t>
+  </si>
+  <si>
+    <t>NOUN, VERB, ADJ</t>
   </si>
 </sst>
 </file>
@@ -492,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97416E94-2161-4DC8-99C4-4B30696C83B6}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -511,7 +493,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -519,10 +501,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -530,10 +512,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -541,10 +523,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -552,10 +534,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -563,10 +545,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -574,10 +556,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -585,10 +567,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
         <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -596,34 +578,32 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated templates xlsx Updated selection of templates to randomly choose one of the available templates given a relation/edgetype
</commit_message>
<xml_diff>
--- a/Data/APNLP_templates.xlsx
+++ b/Data/APNLP_templates.xlsx
@@ -8,12 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elisa\PycharmProjects\Pokerator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D804DC6-F147-45FB-A97B-F686261A14D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85843259-4730-4349-A589-F4277FEF78F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{10266764-591F-4358-9D03-550F328AD39E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="HasA" sheetId="8" r:id="rId2"/>
+    <sheet name="HasProperty" sheetId="9" r:id="rId3"/>
+    <sheet name="PartOf" sheetId="10" r:id="rId4"/>
+    <sheet name="MadeOf" sheetId="11" r:id="rId5"/>
+    <sheet name="AtLocation" sheetId="2" r:id="rId6"/>
+    <sheet name="CapableOf" sheetId="3" r:id="rId7"/>
+    <sheet name="NotDesires" sheetId="4" r:id="rId8"/>
+    <sheet name="Desires" sheetId="5" r:id="rId9"/>
+    <sheet name="UsedFor" sheetId="6" r:id="rId10"/>
+    <sheet name="IsA" sheetId="7" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="45">
   <si>
     <t>Edge types</t>
   </si>
@@ -114,6 +124,60 @@
   </si>
   <si>
     <t>NOUN, VERB, ADJ</t>
+  </si>
+  <si>
+    <t>Its favorite spot is &lt;AtLocation&gt;</t>
+  </si>
+  <si>
+    <t>It likes to be at &lt;AtLocation&gt;</t>
+  </si>
+  <si>
+    <t>In summer, it likes to go to &lt;AtLocation&gt;</t>
+  </si>
+  <si>
+    <t>It likes to hide in &lt;AtLocation&gt;</t>
+  </si>
+  <si>
+    <t>It can &lt;CapableOf&gt;</t>
+  </si>
+  <si>
+    <t>It is capable of &lt;CapableOf&gt;</t>
+  </si>
+  <si>
+    <t>Its favorite thing to do is &lt;CapableOf&gt;</t>
+  </si>
+  <si>
+    <t>Its specialty lies in &lt;CapableOf&gt;</t>
+  </si>
+  <si>
+    <t>It does not desire &lt;NotDesires&gt;</t>
+  </si>
+  <si>
+    <t>It strongly dislikes &lt;NotDesires&gt;</t>
+  </si>
+  <si>
+    <t>It is afraid of &lt;NotDesires&gt;</t>
+  </si>
+  <si>
+    <t>Its least favorite thing is &lt;NotDesires&gt;</t>
+  </si>
+  <si>
+    <t>It loves &lt;Desires&gt;</t>
+  </si>
+  <si>
+    <t>It desires &lt;Desires&gt;</t>
+  </si>
+  <si>
+    <t>Its favorite thing is &lt;Desires&gt;</t>
+  </si>
+  <si>
+    <t>It is especially good at &lt;UsedFor&gt;</t>
+  </si>
+  <si>
+    <t>Its strength lies in &lt;UsedFor&gt;</t>
+  </si>
+  <si>
+    <t>It lives for &lt;Desires&gt;</t>
   </si>
 </sst>
 </file>
@@ -477,7 +541,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -610,4 +674,499 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C53B793-E082-4A0B-8750-ADD51BF59C2F}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.1796875" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12720AB3-91EF-4CF1-8BC0-D254487C04E0}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.7265625" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56C140E-7771-411B-AFB4-39EF6C4A9742}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.90625" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320B7FFD-037D-4A7D-8BA5-5E42AF2E7036}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.6328125" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97CC891B-2CA4-403F-B047-3D1A2AD07BD8}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.08984375" customWidth="1"/>
+    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4ABB0FF-1DE0-4833-9943-8503CCAC83EE}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.36328125" customWidth="1"/>
+    <col min="2" max="2" width="14.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E674BED-8252-4989-9357-F55F3258C74D}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D03F20F2-7003-486E-A633-706225DF8466}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32.54296875" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CF7AE79-6949-4D24-928B-AFECC8CAAAC7}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="28.90625" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25AB0248-1007-4DBB-ABEC-6383C5893342}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.54296875" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>